<commit_message>
Handle (1) Read all entries from all phone books (2) Read all entries from single phone book (3) Create a new phone book entry or update an existing phone book entry
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_Case.xlsx
+++ b/src/test/resources/Test_Case.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/Workspace/Eclipse_Workspace/phone-book/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69703829-2BFA-A049-AAC2-28C9110C4545}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78F7596-2DC3-AD49-8DF0-CF0117B14C1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{51F25B21-A019-3B42-9100-D2CE38A2A811}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Requirement</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Expected result</t>
   </si>
   <si>
-    <t>Actual result</t>
-  </si>
-  <si>
     <t>Two phone books initialized on start up</t>
   </si>
   <si>
@@ -68,25 +65,66 @@
     <t>On starting the console application, there should be 2 phone books initialized</t>
   </si>
   <si>
-    <t>2 phone books are initialized upon console application start up</t>
-  </si>
-  <si>
-    <t>No data should be kept upone console application termination</t>
-  </si>
-  <si>
-    <t>Phone book data is only persisted in memory, and is lost upon termination of application</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>DITTO</t>
-  </si>
-  <si>
-    <t>The phone books show a list of customer s with their phone number</t>
-  </si>
-  <si>
-    <t>The 2 phone books are showing a list of customers and their phone numbers</t>
+    <t>Actual result (dev)</t>
+  </si>
+  <si>
+    <t>Actual result (prod)</t>
+  </si>
+  <si>
+    <t>READ - Users should be able to retrieve all contacts in an address book</t>
+  </si>
+  <si>
+    <t>On quiting, No data should be kept upone console application termination</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Initialisation</t>
+  </si>
+  <si>
+    <t>The phone books show show a list of customers with their phone number</t>
+  </si>
+  <si>
+    <t>Create an entry and no existing entry is found in all phone books.</t>
+  </si>
+  <si>
+    <t>The new entry should be added to the specified phone book only.
+No change to the other phone book.</t>
+  </si>
+  <si>
+    <t>The new number should replace the old number in the specified phone book.
+No change to the other phone book.</t>
+  </si>
+  <si>
+    <t>The new number should replace the old number in the specified phone book.
+The entry in the other phone book should be updated as well.</t>
+  </si>
+  <si>
+    <t>The new entry should be added to the specified phone book.
+The entry in the other phone book should be updated as well.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a new entry where there is already an existing one in the specified phone book.
+The entry does not exist in the other phone book yet.
+</t>
+  </si>
+  <si>
+    <t>Create a new entry where there is already an existing one in the specifed phone book.
+The entry exists in the other phone book as well.</t>
+  </si>
+  <si>
+    <t>Create a new entry where no existing is found in the specifed phone book.
+The entry however exists in the other phone book.</t>
+  </si>
+  <si>
+    <t>Read all entries</t>
+  </si>
+  <si>
+    <t>All entries should be shown for both phone books</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
@@ -142,99 +180,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>5766554</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>5143500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7BE8909-4A1D-0B44-AA3A-C762E3285088}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5388429" y="435429"/>
-          <a:ext cx="5766554" cy="5143500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>5616223</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>5144189</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D4062FA-6B47-0243-9FE7-40F15C6C9A27}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5390444" y="6477000"/>
-          <a:ext cx="5616223" cy="5144189"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -534,90 +479,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7A48FF-9BF2-B64E-BE83-05B901F1C2FC}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="57" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.33203125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="22.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="86.33203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="77.33203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="394" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="153" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Handle read unique set of entries from all phone books
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_Case.xlsx
+++ b/src/test/resources/Test_Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/Workspace/Eclipse_Workspace/phone-book/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78F7596-2DC3-AD49-8DF0-CF0117B14C1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9BC124-28D7-6E48-BC6F-A1F1BBCA4B35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{51F25B21-A019-3B42-9100-D2CE38A2A811}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Requirement</t>
   </si>
@@ -118,13 +118,21 @@
 The entry however exists in the other phone book.</t>
   </si>
   <si>
-    <t>Read all entries</t>
-  </si>
-  <si>
     <t>All entries should be shown for both phone books</t>
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>Read the entries of a specified phone book</t>
+  </si>
+  <si>
+    <t>Read the entries from all phone books.
+Some customers exist in both phone books.</t>
+  </si>
+  <si>
+    <t>A unique set of all entries should be displayed.
+Customers which exist in both phone books should be displayed once only.</t>
   </si>
 </sst>
 </file>
@@ -481,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7A48FF-9BF2-B64E-BE83-05B901F1C2FC}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,7 +533,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -539,7 +547,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="394" customHeight="1" x14ac:dyDescent="0.2">
@@ -553,7 +561,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="408" customHeight="1" x14ac:dyDescent="0.2">
@@ -564,7 +572,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -575,7 +583,7 @@
         <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -586,7 +594,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -594,18 +602,27 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -621,7 +638,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handle delete an entry from single phone book
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_Case.xlsx
+++ b/src/test/resources/Test_Case.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/Workspace/Eclipse_Workspace/phone-book/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9BC124-28D7-6E48-BC6F-A1F1BBCA4B35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE89DFB-2BA5-8B4C-8DFB-B6756BDAD4DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{51F25B21-A019-3B42-9100-D2CE38A2A811}"/>
   </bookViews>
   <sheets>
     <sheet name="Must-Have" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Must-Have'!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Requirement</t>
   </si>
@@ -72,9 +75,6 @@
   </si>
   <si>
     <t>READ - Users should be able to retrieve all contacts in an address book</t>
-  </si>
-  <si>
-    <t>On quiting, No data should be kept upone console application termination</t>
   </si>
   <si>
     <t>Case</t>
@@ -118,13 +118,7 @@
 The entry however exists in the other phone book.</t>
   </si>
   <si>
-    <t>All entries should be shown for both phone books</t>
-  </si>
-  <si>
     <t>Passed</t>
-  </si>
-  <si>
-    <t>Read the entries of a specified phone book</t>
   </si>
   <si>
     <t>Read the entries from all phone books.
@@ -133,6 +127,42 @@
   <si>
     <t>A unique set of all entries should be displayed.
 Customers which exist in both phone books should be displayed once only.</t>
+  </si>
+  <si>
+    <t>All entries should be shown for both phone books.</t>
+  </si>
+  <si>
+    <t>Run application
+Quit application</t>
+  </si>
+  <si>
+    <t>When program is running, data should only be persisting in memory.
+On quiting, no data should be kept in memory or elsewhere (e.g. files)</t>
+  </si>
+  <si>
+    <t>Read the entries of the specified phone book</t>
+  </si>
+  <si>
+    <t>Delete an existing entry from the specified phone book.
+The other phone book also contains the same customer entry.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The entry should be removed from the specified phone book only.
+There should be no change to the other phone book.
+</t>
+  </si>
+  <si>
+    <t>Delete an entry which does not exist in the specified phone book.
+The other phone book does not contain the customer entry as well.</t>
+  </si>
+  <si>
+    <t>Delete an entry which does not exist in the specified phone book.
+The other phone book, however, contains the customer entry.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There should be no change to the specified phone book.
+There should be no change to the other phone book.
+</t>
   </si>
 </sst>
 </file>
@@ -487,10 +517,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7A48FF-9BF2-B64E-BE83-05B901F1C2FC}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -527,13 +560,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -541,13 +574,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="394" customHeight="1" x14ac:dyDescent="0.2">
@@ -555,46 +588,55 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -602,13 +644,13 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -616,32 +658,73 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>26</v>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{49DFC505-6E25-1149-B76C-8F8553D00E05}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add screen operation for "read all entries from all phone books"
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_Case.xlsx
+++ b/src/test/resources/Test_Case.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/Workspace/Eclipse_Workspace/phone-book/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE89DFB-2BA5-8B4C-8DFB-B6756BDAD4DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D84EBAB-D313-9D42-9EB5-11C3F4DDD15E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{51F25B21-A019-3B42-9100-D2CE38A2A811}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{51F25B21-A019-3B42-9100-D2CE38A2A811}"/>
   </bookViews>
   <sheets>
     <sheet name="Must-Have" sheetId="1" r:id="rId1"/>
+    <sheet name="Extra" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Extra!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Must-Have'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>Requirement</t>
   </si>
@@ -163,6 +165,66 @@
     <t xml:space="preserve">There should be no change to the specified phone book.
 There should be no change to the other phone book.
 </t>
+  </si>
+  <si>
+    <t>READ - Users should be able to retrieve all contacts in an address book	Read the entries from all phone books</t>
+  </si>
+  <si>
+    <t>All entries from all phone books should be shown</t>
+  </si>
+  <si>
+    <t>Read the entries from all phone books</t>
+  </si>
+  <si>
+    <t>RESTful API endpoint for createEntry</t>
+  </si>
+  <si>
+    <t>RESTful API endpoint for updateEntry</t>
+  </si>
+  <si>
+    <t>RESTful API endpoint for readAllEntriesFromAllPhoneBooks</t>
+  </si>
+  <si>
+    <t>RESTful API endpoint for readAllEntriesFromSinglePhoneBook</t>
+  </si>
+  <si>
+    <t>RESTful API endpoint for readUniqueEntriesFromAllPhoneBooks</t>
+  </si>
+  <si>
+    <t>RESTful API endpoint for deleteEntryFromSinglePhoneBook</t>
+  </si>
+  <si>
+    <t>A message should be returned indicating the successful creation of the entry</t>
+  </si>
+  <si>
+    <t>A message should be returned indicating the successful update of the entry</t>
+  </si>
+  <si>
+    <t>A list containing all phone book entries should be returned</t>
+  </si>
+  <si>
+    <t>Create a new customer entry in the specified phone book</t>
+  </si>
+  <si>
+    <t>Update an existing customer entry in the specified phone book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read the entries from the specified phone book </t>
+  </si>
+  <si>
+    <t>The phoneBook entries of the specified phone book should be returned</t>
+  </si>
+  <si>
+    <t>Read unique entries across all phone books</t>
+  </si>
+  <si>
+    <t>Unique entires from across all phone books should be returned</t>
+  </si>
+  <si>
+    <t>Delete an existing entry from the specified phone book.</t>
+  </si>
+  <si>
+    <t>The entry should be removed from the specified phone book</t>
   </si>
 </sst>
 </file>
@@ -519,11 +581,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7A48FF-9BF2-B64E-BE83-05B901F1C2FC}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,4 +789,145 @@
   <autoFilter ref="A1:F1" xr:uid="{49DFC505-6E25-1149-B76C-8F8553D00E05}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5A0118-ED37-B449-A081-9B606FAE81A3}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="136" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="136" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="136" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{EC021ED4-3B00-1948-B490-D57A6D09EE6B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>